<commit_message>
add support for reading empty cell and row
</commit_message>
<xml_diff>
--- a/testImport2/Book1.xlsx
+++ b/testImport2/Book1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mygo\src\github.com\kharism\effectiveexport\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mygo\src\github.com\eaciit\hoboexcel\testImport2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>row 1 b</t>
   </si>
@@ -84,14 +84,59 @@
   </si>
   <si>
     <t>row 2 j</t>
+  </si>
+  <si>
+    <t>utf</t>
+  </si>
+  <si>
+    <t>日本語</t>
+  </si>
+  <si>
+    <t>bold</t>
+  </si>
+  <si>
+    <t>italic</t>
+  </si>
+  <si>
+    <t>underline</t>
+  </si>
+  <si>
+    <t>Jump Row</t>
+  </si>
+  <si>
+    <t>Another Row</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -119,8 +164,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,7 +554,35 @@
         <v>70.61999999999999</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>